<commit_message>
done download excel setup ck4
</commit_message>
<xml_diff>
--- a/src/templateFiles/template_ck4_mmea.xlsx
+++ b/src/templateFiles/template_ck4_mmea.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="11110" windowHeight="7390"/>
+    <workbookView windowWidth="15420" windowHeight="6830"/>
   </bookViews>
   <sheets>
     <sheet name="APR 2023" sheetId="3" r:id="rId1"/>
@@ -53,12 +53,11 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9">
-  <numFmts count="5">
+  <numFmts count="4">
     <numFmt numFmtId="176" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="177" formatCode="_-&quot;Rp&quot;* #,##0.00_-;\-&quot;Rp&quot;* #,##0.00_-;_-&quot;Rp&quot;* &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="178" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;_);_(@_)"/>
     <numFmt numFmtId="179" formatCode="_-&quot;Rp&quot;* #,##0_-;\-&quot;Rp&quot;* #,##0_-;_-&quot;Rp&quot;* &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="180" formatCode="dd/mm/yyyy;@"/>
   </numFmts>
   <fonts count="20">
     <font>
@@ -661,10 +660,9 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="58" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="180" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="49">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -984,10 +982,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:K115"/>
+  <dimension ref="A1:K1"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="F3" sqref="F3"/>
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.5"/>
@@ -1040,348 +1038,6 @@
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="8:8">
-      <c r="H2" s="2"/>
-    </row>
-    <row r="3" spans="8:8">
-      <c r="H3" s="2"/>
-    </row>
-    <row r="4" spans="8:8">
-      <c r="H4" s="2"/>
-    </row>
-    <row r="5" spans="8:8">
-      <c r="H5" s="2"/>
-    </row>
-    <row r="6" spans="8:8">
-      <c r="H6" s="2"/>
-    </row>
-    <row r="7" spans="8:8">
-      <c r="H7" s="2"/>
-    </row>
-    <row r="8" spans="8:8">
-      <c r="H8" s="2"/>
-    </row>
-    <row r="9" spans="8:8">
-      <c r="H9" s="2"/>
-    </row>
-    <row r="10" spans="8:8">
-      <c r="H10" s="2"/>
-    </row>
-    <row r="11" spans="8:8">
-      <c r="H11" s="2"/>
-    </row>
-    <row r="12" spans="8:8">
-      <c r="H12" s="2"/>
-    </row>
-    <row r="13" spans="8:8">
-      <c r="H13" s="2"/>
-    </row>
-    <row r="14" spans="8:8">
-      <c r="H14" s="2"/>
-    </row>
-    <row r="15" spans="8:8">
-      <c r="H15" s="2"/>
-    </row>
-    <row r="16" spans="8:8">
-      <c r="H16" s="2"/>
-    </row>
-    <row r="17" spans="8:8">
-      <c r="H17" s="2"/>
-    </row>
-    <row r="18" spans="8:8">
-      <c r="H18" s="2"/>
-    </row>
-    <row r="19" spans="8:8">
-      <c r="H19" s="2"/>
-    </row>
-    <row r="20" spans="8:8">
-      <c r="H20" s="2"/>
-    </row>
-    <row r="21" spans="8:8">
-      <c r="H21" s="2"/>
-    </row>
-    <row r="22" spans="8:8">
-      <c r="H22" s="2"/>
-    </row>
-    <row r="23" spans="8:8">
-      <c r="H23" s="2"/>
-    </row>
-    <row r="24" spans="8:8">
-      <c r="H24" s="2"/>
-    </row>
-    <row r="25" spans="8:8">
-      <c r="H25" s="2"/>
-    </row>
-    <row r="26" spans="8:8">
-      <c r="H26" s="2"/>
-    </row>
-    <row r="27" spans="8:8">
-      <c r="H27" s="2"/>
-    </row>
-    <row r="28" spans="8:8">
-      <c r="H28" s="2"/>
-    </row>
-    <row r="29" spans="8:8">
-      <c r="H29" s="2"/>
-    </row>
-    <row r="30" spans="8:8">
-      <c r="H30" s="2"/>
-    </row>
-    <row r="31" spans="8:8">
-      <c r="H31" s="2"/>
-    </row>
-    <row r="32" spans="8:8">
-      <c r="H32" s="2"/>
-    </row>
-    <row r="33" spans="8:8">
-      <c r="H33" s="2"/>
-    </row>
-    <row r="34" spans="8:8">
-      <c r="H34" s="2"/>
-    </row>
-    <row r="35" spans="8:8">
-      <c r="H35" s="2"/>
-    </row>
-    <row r="36" spans="8:8">
-      <c r="H36" s="2"/>
-    </row>
-    <row r="37" spans="8:8">
-      <c r="H37" s="2"/>
-    </row>
-    <row r="38" spans="8:8">
-      <c r="H38" s="2"/>
-    </row>
-    <row r="39" spans="8:8">
-      <c r="H39" s="2"/>
-    </row>
-    <row r="40" spans="8:8">
-      <c r="H40" s="2"/>
-    </row>
-    <row r="41" spans="8:8">
-      <c r="H41" s="2"/>
-    </row>
-    <row r="42" spans="8:8">
-      <c r="H42" s="2"/>
-    </row>
-    <row r="43" spans="8:8">
-      <c r="H43" s="2"/>
-    </row>
-    <row r="44" spans="8:8">
-      <c r="H44" s="2"/>
-    </row>
-    <row r="45" spans="8:8">
-      <c r="H45" s="2"/>
-    </row>
-    <row r="46" spans="8:8">
-      <c r="H46" s="2"/>
-    </row>
-    <row r="47" spans="8:8">
-      <c r="H47" s="2"/>
-    </row>
-    <row r="48" spans="8:8">
-      <c r="H48" s="2"/>
-    </row>
-    <row r="49" spans="8:8">
-      <c r="H49" s="2"/>
-    </row>
-    <row r="50" spans="8:8">
-      <c r="H50" s="2"/>
-    </row>
-    <row r="51" spans="8:8">
-      <c r="H51" s="2"/>
-    </row>
-    <row r="52" spans="8:8">
-      <c r="H52" s="2"/>
-    </row>
-    <row r="53" spans="8:8">
-      <c r="H53" s="2"/>
-    </row>
-    <row r="54" spans="8:8">
-      <c r="H54" s="2"/>
-    </row>
-    <row r="55" spans="8:8">
-      <c r="H55" s="2"/>
-    </row>
-    <row r="56" spans="8:8">
-      <c r="H56" s="2"/>
-    </row>
-    <row r="57" spans="8:8">
-      <c r="H57" s="2"/>
-    </row>
-    <row r="58" spans="8:8">
-      <c r="H58" s="2"/>
-    </row>
-    <row r="59" spans="8:8">
-      <c r="H59" s="2"/>
-    </row>
-    <row r="60" spans="8:8">
-      <c r="H60" s="2"/>
-    </row>
-    <row r="61" spans="8:8">
-      <c r="H61" s="2"/>
-    </row>
-    <row r="62" spans="8:8">
-      <c r="H62" s="2"/>
-    </row>
-    <row r="63" spans="8:8">
-      <c r="H63" s="2"/>
-    </row>
-    <row r="64" spans="8:8">
-      <c r="H64" s="2"/>
-    </row>
-    <row r="65" spans="8:8">
-      <c r="H65" s="2"/>
-    </row>
-    <row r="66" spans="8:8">
-      <c r="H66" s="2"/>
-    </row>
-    <row r="67" spans="8:8">
-      <c r="H67" s="2"/>
-    </row>
-    <row r="68" spans="8:8">
-      <c r="H68" s="2"/>
-    </row>
-    <row r="69" spans="8:8">
-      <c r="H69" s="2"/>
-    </row>
-    <row r="70" spans="8:8">
-      <c r="H70" s="2"/>
-    </row>
-    <row r="71" spans="8:8">
-      <c r="H71" s="1"/>
-    </row>
-    <row r="72" spans="8:8">
-      <c r="H72" s="1"/>
-    </row>
-    <row r="73" spans="8:8">
-      <c r="H73" s="1"/>
-    </row>
-    <row r="74" spans="8:8">
-      <c r="H74" s="1"/>
-    </row>
-    <row r="75" spans="8:8">
-      <c r="H75" s="1"/>
-    </row>
-    <row r="76" spans="8:8">
-      <c r="H76" s="1"/>
-    </row>
-    <row r="77" spans="8:8">
-      <c r="H77" s="1"/>
-    </row>
-    <row r="78" spans="8:8">
-      <c r="H78" s="1"/>
-    </row>
-    <row r="79" spans="8:8">
-      <c r="H79" s="1"/>
-    </row>
-    <row r="80" spans="8:8">
-      <c r="H80" s="1"/>
-    </row>
-    <row r="81" spans="8:8">
-      <c r="H81" s="1"/>
-    </row>
-    <row r="82" spans="8:8">
-      <c r="H82" s="1"/>
-    </row>
-    <row r="83" spans="8:8">
-      <c r="H83" s="1"/>
-    </row>
-    <row r="84" spans="8:8">
-      <c r="H84" s="1"/>
-    </row>
-    <row r="85" spans="8:8">
-      <c r="H85" s="1"/>
-    </row>
-    <row r="86" spans="8:8">
-      <c r="H86" s="1"/>
-    </row>
-    <row r="87" spans="8:8">
-      <c r="H87" s="1"/>
-    </row>
-    <row r="88" spans="8:8">
-      <c r="H88" s="1"/>
-    </row>
-    <row r="89" spans="8:8">
-      <c r="H89" s="1"/>
-    </row>
-    <row r="90" spans="8:8">
-      <c r="H90" s="1"/>
-    </row>
-    <row r="91" spans="8:8">
-      <c r="H91" s="1"/>
-    </row>
-    <row r="92" spans="8:8">
-      <c r="H92" s="1"/>
-    </row>
-    <row r="93" spans="8:8">
-      <c r="H93" s="1"/>
-    </row>
-    <row r="94" spans="8:8">
-      <c r="H94" s="1"/>
-    </row>
-    <row r="95" spans="8:8">
-      <c r="H95" s="1"/>
-    </row>
-    <row r="96" spans="8:8">
-      <c r="H96" s="1"/>
-    </row>
-    <row r="97" spans="8:8">
-      <c r="H97" s="1"/>
-    </row>
-    <row r="98" spans="8:8">
-      <c r="H98" s="1"/>
-    </row>
-    <row r="99" spans="8:8">
-      <c r="H99" s="1"/>
-    </row>
-    <row r="100" spans="8:8">
-      <c r="H100" s="1"/>
-    </row>
-    <row r="101" spans="8:8">
-      <c r="H101" s="1"/>
-    </row>
-    <row r="102" spans="8:8">
-      <c r="H102" s="1"/>
-    </row>
-    <row r="103" spans="8:8">
-      <c r="H103" s="1"/>
-    </row>
-    <row r="104" spans="8:8">
-      <c r="H104" s="1"/>
-    </row>
-    <row r="105" spans="8:8">
-      <c r="H105" s="1"/>
-    </row>
-    <row r="106" spans="8:8">
-      <c r="H106" s="1"/>
-    </row>
-    <row r="107" spans="8:8">
-      <c r="H107" s="1"/>
-    </row>
-    <row r="108" spans="8:8">
-      <c r="H108" s="1"/>
-    </row>
-    <row r="109" spans="8:8">
-      <c r="H109" s="1"/>
-    </row>
-    <row r="110" spans="8:8">
-      <c r="H110" s="1"/>
-    </row>
-    <row r="111" spans="8:8">
-      <c r="H111" s="1"/>
-    </row>
-    <row r="112" spans="8:8">
-      <c r="H112" s="1"/>
-    </row>
-    <row r="113" spans="8:8">
-      <c r="H113" s="1"/>
-    </row>
-    <row r="114" spans="8:8">
-      <c r="H114" s="1"/>
-    </row>
-    <row r="115" spans="8:8">
-      <c r="H115" s="1"/>
-    </row>
   </sheetData>
   <pageMargins left="0" right="0" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="5" scale="70" orientation="portrait"/>

</xml_diff>